<commit_message>
Added attack and giveDamage to Monster class.  Initial attempt at balanced combat probabilities.  See spreadsheet for details in calculations.
</commit_message>
<xml_diff>
--- a/dev_documents/Test_Values.xlsx
+++ b/dev_documents/Test_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nerd\School\Spring_2021\CS_143_Java_II\Stalactite_Fight_Night\stalactite_fight_night\dev_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1FD5C0-6882-42F7-BFB5-2D682F624C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA5657-03FC-426C-A929-E7D6E60031E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="315" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Level</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Monster STR</t>
+  </si>
+  <si>
+    <t>Monster STR to hit</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +460,9 @@
       <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -499,6 +504,10 @@
         <f>A2+9</f>
         <v>10</v>
       </c>
+      <c r="M2" s="1">
+        <f>A2-ROUND(L2/7, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -540,13 +549,17 @@
         <f t="shared" ref="L3:L40" si="4">A3+9</f>
         <v>11</v>
       </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:M40" si="5">A3-ROUND(L3/7, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B40" si="5">B3+(3*J3)</f>
+        <f t="shared" ref="B4:B40" si="6">B3+(3*J3)</f>
         <v>126</v>
       </c>
       <c r="C4" s="1">
@@ -580,6 +593,10 @@
       <c r="L4" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
+      </c>
+      <c r="M4" s="1">
+        <f>A4-ROUND(L4/7, 0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -587,7 +604,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>207</v>
       </c>
       <c r="C5" s="1">
@@ -621,6 +638,10 @@
       <c r="L5" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -628,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>306</v>
       </c>
       <c r="C6" s="1">
@@ -662,6 +683,10 @@
       <c r="L6" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -669,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>414</v>
       </c>
       <c r="C7" s="1">
@@ -703,6 +728,10 @@
       <c r="L7" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -710,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>540</v>
       </c>
       <c r="C8" s="1">
@@ -744,6 +773,10 @@
       <c r="L8" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -751,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>675</v>
       </c>
       <c r="C9" s="1">
@@ -785,6 +818,10 @@
       <c r="L9" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -792,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>828</v>
       </c>
       <c r="C10" s="1">
@@ -826,6 +863,10 @@
       <c r="L10" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -833,7 +874,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>990</v>
       </c>
       <c r="C11" s="1">
@@ -867,6 +908,10 @@
       <c r="L11" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -874,7 +919,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1170</v>
       </c>
       <c r="C12" s="1">
@@ -908,6 +953,10 @@
       <c r="L12" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -915,7 +964,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1359</v>
       </c>
       <c r="C13" s="1">
@@ -949,6 +998,10 @@
       <c r="L13" s="1">
         <f t="shared" si="4"/>
         <v>21</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -956,7 +1009,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1566</v>
       </c>
       <c r="C14" s="1">
@@ -990,6 +1043,10 @@
       <c r="L14" s="1">
         <f t="shared" si="4"/>
         <v>22</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -997,7 +1054,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1782</v>
       </c>
       <c r="C15" s="1">
@@ -1031,6 +1088,10 @@
       <c r="L15" s="1">
         <f t="shared" si="4"/>
         <v>23</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1038,7 +1099,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2016</v>
       </c>
       <c r="C16" s="1">
@@ -1073,13 +1134,17 @@
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="1">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2259</v>
       </c>
       <c r="C17" s="1">
@@ -1114,13 +1179,17 @@
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="1">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2520</v>
       </c>
       <c r="C18" s="1">
@@ -1155,13 +1224,17 @@
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="1">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2790</v>
       </c>
       <c r="C19" s="1">
@@ -1196,13 +1269,17 @@
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="1">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3078</v>
       </c>
       <c r="C20" s="1">
@@ -1237,13 +1314,17 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="1">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3375</v>
       </c>
       <c r="C21" s="1">
@@ -1278,13 +1359,17 @@
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="1">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3690</v>
       </c>
       <c r="C22" s="1">
@@ -1319,13 +1404,17 @@
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="1">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4014</v>
       </c>
       <c r="C23" s="1">
@@ -1360,13 +1449,17 @@
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="1">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4356</v>
       </c>
       <c r="C24" s="1">
@@ -1401,13 +1494,17 @@
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="1">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4707</v>
       </c>
       <c r="C25" s="1">
@@ -1442,13 +1539,17 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="1">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5076</v>
       </c>
       <c r="C26" s="1">
@@ -1483,13 +1584,17 @@
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="1">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5454</v>
       </c>
       <c r="C27" s="1">
@@ -1524,13 +1629,17 @@
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="1">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5850</v>
       </c>
       <c r="C28" s="1">
@@ -1565,13 +1674,17 @@
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="1">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6255</v>
       </c>
       <c r="C29" s="1">
@@ -1606,13 +1719,17 @@
         <f t="shared" si="4"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="1">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6678</v>
       </c>
       <c r="C30" s="1">
@@ -1647,13 +1764,17 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="1">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7110</v>
       </c>
       <c r="C31" s="1">
@@ -1688,13 +1809,17 @@
         <f t="shared" si="4"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="1">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7560</v>
       </c>
       <c r="C32" s="1">
@@ -1729,13 +1854,17 @@
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" s="1">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8019</v>
       </c>
       <c r="C33" s="1">
@@ -1770,13 +1899,17 @@
         <f t="shared" si="4"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" s="1">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8496</v>
       </c>
       <c r="C34" s="1">
@@ -1811,13 +1944,17 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" s="1">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8982</v>
       </c>
       <c r="C35" s="1">
@@ -1852,13 +1989,17 @@
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="1">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9486</v>
       </c>
       <c r="C36" s="1">
@@ -1893,13 +2034,17 @@
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="1">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9999</v>
       </c>
       <c r="C37" s="1">
@@ -1934,13 +2079,17 @@
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="1">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10530</v>
       </c>
       <c r="C38" s="1">
@@ -1975,13 +2124,17 @@
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="1">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11070</v>
       </c>
       <c r="C39" s="1">
@@ -2016,13 +2169,17 @@
         <f t="shared" si="4"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="1">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11628</v>
       </c>
       <c r="C40" s="1">
@@ -2056,6 +2213,10 @@
       <c r="L40" s="1">
         <f t="shared" si="4"/>
         <v>48</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="5"/>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added attack and giveDamage for Adventurer, including interface with Armor and Weapon classes.
</commit_message>
<xml_diff>
--- a/dev_documents/Test_Values.xlsx
+++ b/dev_documents/Test_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nerd\School\Spring_2021\CS_143_Java_II\Stalactite_Fight_Night\stalactite_fight_night\dev_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA5657-03FC-426C-A929-E7D6E60031E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E5D1F-3FBB-4C1A-89E3-9FBFFC41B29D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="315" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,7 +432,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,9 +494,9 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <f>(ROUND((9+A2)/2,0) + A2)*4</f>
-        <v>24</v>
+      <c r="C2" s="1" t="e" cm="1">
+        <f t="array" ref="C2">(ROUND((9+A2)/2,0) + P21A2)*4</f>
+        <v>#NAME?</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>

</xml_diff>

<commit_message>
Significantly streamlined function to read in values from files
</commit_message>
<xml_diff>
--- a/dev_documents/Test_Values.xlsx
+++ b/dev_documents/Test_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nerd\School\Spring_2021\CS_143_Java_II\Stalactite_Fight_Night\stalactite_fight_night\dev_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E5D1F-3FBB-4C1A-89E3-9FBFFC41B29D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232464D1-AE49-4D2E-8316-C40EDD743FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="315" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,28 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,7 +410,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,9 +472,9 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="e" cm="1">
-        <f t="array" ref="C2">(ROUND((9+A2)/2,0) + P21A2)*4</f>
-        <v>#NAME?</v>
+      <c r="C2" s="1">
+        <f>(ROUND((9+A2)/2,0) +A2)*4</f>
+        <v>24</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>

</xml_diff>